<commit_message>
format barcode di dokumentasi
</commit_message>
<xml_diff>
--- a/public/assets/product.xlsx
+++ b/public/assets/product.xlsx
@@ -86,9 +86,6 @@
     <t>Deskripsi Produk B</t>
   </si>
   <si>
-    <t>ean</t>
-  </si>
-  <si>
     <t>Produk A baru sekali</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>ean13</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" activeCellId="1" sqref="M1:O1 M6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -446,7 +446,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -496,7 +496,7 @@
         <v>1205</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>10000</v>
@@ -514,7 +514,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J2">
         <v>10</v>
@@ -540,7 +540,7 @@
         <v>1206</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>10002</v>
@@ -558,7 +558,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J3">
         <v>20</v>

</xml_diff>